<commit_message>
change C to FCU
</commit_message>
<xml_diff>
--- a/MODERN MECHANICS/Lab_1_sheet.xlsx
+++ b/MODERN MECHANICS/Lab_1_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonsici/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDDD0B8D-D47A-004C-9041-32E896F6AF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667E72A0-EA76-7542-B6A6-EE7C0BBD0818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D1E6293E-CBD8-FE4C-B351-DC7263C59724}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +60,22 @@
   </si>
   <si>
     <t>AVR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -97,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -105,13 +121,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -127,7 +223,49 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,465 +582,575 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D73E76-A42D-A048-B705-3827523D4B7B}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="200" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="3" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="11.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7"/>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>22.2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>31.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
+      <c r="E3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>0.38600000000000001</v>
       </c>
-      <c r="E3" s="5">
-        <f>B35-2.5 * B36</f>
+      <c r="E4" s="14">
+        <f>B36-2.5 * B37</f>
         <v>0.51859953168259176</v>
       </c>
-      <c r="F3" s="5">
-        <f>B35-1.5 * B36 - 0.001</f>
+      <c r="F4" s="15">
+        <f>B36-1.5 * B37 - 0.001</f>
         <v>0.52915971900955505</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
+      <c r="G4" s="16">
+        <f t="array" ref="G4:G8">FREQUENCY(B4:B33,F4:F8)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.54700000000000004</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>0.375</v>
       </c>
-      <c r="E4" s="5">
-        <f>B35-1.5 * B36</f>
+      <c r="E5" s="14">
+        <f>B36-1.5 * B37</f>
         <v>0.53015971900955505</v>
       </c>
-      <c r="F4" s="5">
-        <f>B35-0.5 * B36 - 0.001</f>
+      <c r="F5" s="15">
+        <f>B36-0.5 * B37 - 0.001</f>
         <v>0.54071990633651834</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
+      <c r="G5" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>0.53300000000000003</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>0.373</v>
       </c>
-      <c r="E5" s="5">
-        <f>B35-0.5 * B36</f>
+      <c r="E6" s="14">
+        <f>B36-0.5 * B37</f>
         <v>0.54171990633651834</v>
       </c>
-      <c r="F5" s="5">
-        <f>B35+0.5 * B36 - 0.001</f>
+      <c r="F6" s="15">
+        <f>B36+0.5 * B37 - 0.001</f>
         <v>0.55228009366348163</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
+      <c r="G6" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>0.38200000000000001</v>
       </c>
-      <c r="E6" s="5">
-        <f>B35+0.5 * B36</f>
+      <c r="E7" s="14">
+        <f>B36+0.5 * B37</f>
         <v>0.55328009366348163</v>
       </c>
-      <c r="F6" s="5">
-        <f>B35+1.5 * B36 - 0.001</f>
+      <c r="F7" s="15">
+        <f>B36+1.5 * B37 - 0.001</f>
         <v>0.56384028099044492</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3">
+      <c r="G7" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>0.57199999999999995</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>0.41199999999999998</v>
       </c>
-      <c r="E7" s="5">
-        <f>B35+1.5 * B36</f>
+      <c r="E8" s="17">
+        <f>B36+1.5 * B37</f>
         <v>0.56484028099044492</v>
       </c>
-      <c r="F7" s="5">
-        <f>B35+2.5 * B36</f>
+      <c r="F8" s="18">
+        <f>B36+2.5 * B37</f>
         <v>0.57640046831740821</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3">
+      <c r="G8" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>0.433</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3">
+    <row r="10" spans="1:7">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>0.56200000000000006</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3">
+      <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
         <v>0.53900000000000003</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>0.39600000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3">
+      <c r="E11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="F11" s="12"/>
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
         <v>0.55200000000000005</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>0.39900000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3">
+      <c r="E12" s="14">
+        <f>C36-2.5 * C37</f>
+        <v>0.36949328987222013</v>
+      </c>
+      <c r="F12" s="15">
+        <f>C36-1.5 * C37 - 0.001</f>
+        <v>0.38188264058999871</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="array" ref="G12:G16">FREQUENCY(C4:C33,F12:F16)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>0.56599999999999995</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>0.39600000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3">
+      <c r="E13" s="14">
+        <f>C36-1.5 * C37</f>
+        <v>0.38288264058999871</v>
+      </c>
+      <c r="F13" s="15">
+        <f>C36-0.5 * C37 - 0.001</f>
+        <v>0.39527199130777729</v>
+      </c>
+      <c r="G13" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>0.54400000000000004</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>0.40699999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3">
+      <c r="E14" s="14">
+        <f>C36-0.5 * C37</f>
+        <v>0.39627199130777729</v>
+      </c>
+      <c r="F14" s="15">
+        <f>C36+0.5 * C37 - 0.001</f>
+        <v>0.40866134202555587</v>
+      </c>
+      <c r="G14" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>0.54700000000000004</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>0.39100000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3">
+      <c r="E15" s="14">
+        <f>C36+0.5 * C37</f>
+        <v>0.40966134202555587</v>
+      </c>
+      <c r="F15" s="15">
+        <f>C36+1.5 * C37 - 0.001</f>
+        <v>0.42205069274333445</v>
+      </c>
+      <c r="G15" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.40899999999999997</v>
+      <c r="E16" s="17">
+        <f>C36+1.5 * C37</f>
+        <v>0.42305069274333446</v>
+      </c>
+      <c r="F16" s="18">
+        <f>C36+2.5 * C37</f>
+        <v>0.43644004346111304</v>
+      </c>
+      <c r="G16" s="19">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
-        <v>0.54900000000000004</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="C17" s="1">
-        <v>0.40200000000000002</v>
+        <v>0.40899999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
-        <v>0.55300000000000005</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="C18" s="1">
-        <v>0.40799999999999997</v>
+        <v>0.40200000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>0.54300000000000004</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="C19" s="1">
-        <v>0.40699999999999997</v>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>0.55100000000000005</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="C20" s="1">
-        <v>0.39400000000000002</v>
+        <v>0.40699999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1">
-        <v>0.54200000000000004</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="C21" s="1">
-        <v>0.39800000000000002</v>
+        <v>0.39400000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1">
-        <v>0.53800000000000003</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="C22" s="1">
-        <v>0.42399999999999999</v>
+        <v>0.39800000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
-        <v>0.52900000000000003</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="C23" s="1">
-        <v>0.40699999999999997</v>
+        <v>0.42399999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1">
-        <v>0.52800000000000002</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="C24" s="1">
-        <v>0.41499999999999998</v>
+        <v>0.40699999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>0.53900000000000003</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="C25" s="1">
-        <v>0.40699999999999997</v>
+        <v>0.41499999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>0.53500000000000003</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="C26" s="1">
-        <v>0.42099999999999999</v>
+        <v>0.40699999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1">
-        <v>0.54700000000000004</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="C27" s="1">
-        <v>0.41899999999999998</v>
+        <v>0.42099999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1">
-        <v>0.54900000000000004</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="C28" s="1">
-        <v>0.41</v>
+        <v>0.41899999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1">
-        <v>0.53700000000000003</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="C29" s="1">
-        <v>0.40799999999999997</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1">
-        <v>0.54900000000000004</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="C30" s="1">
-        <v>0.40200000000000002</v>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1">
-        <v>0.54500000000000004</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="C31" s="1">
-        <v>0.40100000000000002</v>
+        <v>0.40200000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.40100000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B33" s="1">
         <v>0.54100000000000004</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>0.40899999999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1">
-        <f>MAX(B3:B32)</f>
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="C33" s="1">
-        <f>MAX(C3:C32)</f>
-        <v>0.433</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1">
-        <f>MIN(B3:B32)</f>
-        <v>0.52800000000000002</v>
+        <f>MAX(B4:B33)</f>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C34" s="1">
-        <f>MIN(C3:C32)</f>
-        <v>0.373</v>
+        <f>MAX(C4:C33)</f>
+        <v>0.433</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B35" s="1">
-        <f xml:space="preserve"> AVERAGE(B3:B32)</f>
-        <v>0.54749999999999999</v>
+        <f>MIN(B4:B33)</f>
+        <v>0.52800000000000002</v>
       </c>
       <c r="C35" s="1">
-        <f xml:space="preserve"> AVERAGE(C3:C32)</f>
-        <v>0.40296666666666658</v>
+        <f>MIN(C4:C33)</f>
+        <v>0.373</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1">
+        <f xml:space="preserve"> AVERAGE(B4:B33)</f>
+        <v>0.54749999999999999</v>
+      </c>
+      <c r="C36" s="1">
+        <f xml:space="preserve"> AVERAGE(C4:C33)</f>
+        <v>0.40296666666666658</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="1">
-        <f>STDEV(B3:B32)</f>
+      <c r="B37" s="1">
+        <f>STDEV(B4:B33)</f>
         <v>1.1560187326963275E-2</v>
       </c>
-      <c r="C36" s="1">
-        <f>STDEV(C3:C32)</f>
+      <c r="C37" s="1">
+        <f>STDEV(C4:C33)</f>
         <v>1.3389350717778583E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>